<commit_message>
added inline documentation and some changes to text on app
</commit_message>
<xml_diff>
--- a/finalApp/input_data/state_climate_zone.xlsx
+++ b/finalApp/input_data/state_climate_zone.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganty/Desktop/current_projects/energy_price_app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganty/energy_price_app/finalApp/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BF79DC-5CEC-BB4D-AD8C-C9A096735CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEE53C2-9284-8545-8186-8FB1026D9287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21660" yWindow="2100" windowWidth="15080" windowHeight="18200" xr2:uid="{F0F0F14D-5213-5F4F-9A78-8932333C0828}"/>
+    <workbookView xWindow="21660" yWindow="1980" windowWidth="15080" windowHeight="18200" xr2:uid="{F0F0F14D-5213-5F4F-9A78-8932333C0828}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="61">
   <si>
     <t>state</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>Marine</t>
-  </si>
-  <si>
-    <t>Coastal CA</t>
   </si>
 </sst>
 </file>
@@ -297,14 +294,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -629,19 +625,19 @@
   <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
@@ -649,7 +645,7 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -657,7 +653,7 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -665,7 +661,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -673,15 +669,15 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -689,7 +685,7 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -697,7 +693,7 @@
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -705,7 +701,7 @@
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -713,15 +709,15 @@
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>60</v>
       </c>
     </row>
@@ -729,7 +725,7 @@
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -737,7 +733,7 @@
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -745,7 +741,7 @@
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>59</v>
       </c>
     </row>
@@ -753,7 +749,7 @@
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -761,7 +757,7 @@
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -769,7 +765,7 @@
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -777,7 +773,7 @@
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -785,7 +781,7 @@
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -793,7 +789,7 @@
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -801,7 +797,7 @@
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -809,7 +805,7 @@
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -817,7 +813,7 @@
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -825,7 +821,7 @@
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -833,7 +829,7 @@
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -841,7 +837,7 @@
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -849,7 +845,7 @@
       <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -857,7 +853,7 @@
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -865,7 +861,7 @@
       <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -873,7 +869,7 @@
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -881,7 +877,7 @@
       <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -889,7 +885,7 @@
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -897,7 +893,7 @@
       <c r="A33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -905,7 +901,7 @@
       <c r="A34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -913,7 +909,7 @@
       <c r="A35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -921,7 +917,7 @@
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -929,7 +925,7 @@
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -937,7 +933,7 @@
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -945,7 +941,7 @@
       <c r="A39" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -953,7 +949,7 @@
       <c r="A40" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -961,7 +957,7 @@
       <c r="A41" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -969,7 +965,7 @@
       <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -977,7 +973,7 @@
       <c r="A43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>59</v>
       </c>
     </row>
@@ -985,7 +981,7 @@
       <c r="A44" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -993,7 +989,7 @@
       <c r="A45" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1001,7 +997,7 @@
       <c r="A46" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1009,7 +1005,7 @@
       <c r="A47" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1017,7 +1013,7 @@
       <c r="A48" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1025,7 +1021,7 @@
       <c r="A49" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1033,7 +1029,7 @@
       <c r="A50" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1041,7 +1037,7 @@
       <c r="A51" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1049,7 +1045,7 @@
       <c r="A52" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1057,7 +1053,7 @@
       <c r="A53" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1065,7 +1061,7 @@
       <c r="A54" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1073,7 +1069,7 @@
       <c r="A55" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1081,7 +1077,7 @@
       <c r="A56" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1089,7 +1085,7 @@
       <c r="A57" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1097,7 +1093,7 @@
       <c r="A58" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1105,7 +1101,7 @@
       <c r="A59" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="4" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1113,7 +1109,7 @@
       <c r="A60" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1121,7 +1117,7 @@
       <c r="A61" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1129,7 +1125,7 @@
       <c r="A62" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1137,7 +1133,7 @@
       <c r="A63" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1145,7 +1141,7 @@
       <c r="A64" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1153,7 +1149,7 @@
       <c r="A65" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1161,7 +1157,7 @@
       <c r="A66" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1169,7 +1165,7 @@
       <c r="A67" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1177,7 +1173,7 @@
       <c r="A68" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1185,7 +1181,7 @@
       <c r="A69" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1193,7 +1189,7 @@
       <c r="A70" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1201,7 +1197,7 @@
       <c r="A71" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1209,7 +1205,7 @@
       <c r="A72" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1217,7 +1213,7 @@
       <c r="A73" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1225,7 +1221,7 @@
       <c r="A74" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="4" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1233,7 +1229,7 @@
       <c r="A75" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1241,7 +1237,7 @@
       <c r="A76" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1249,7 +1245,7 @@
       <c r="A77" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1257,7 +1253,7 @@
       <c r="A78" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1265,7 +1261,7 @@
       <c r="A79" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="4" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>